<commit_message>
Updated dev tasks for use case 3 - Near store activity
</commit_message>
<xml_diff>
--- a/docs/DevTasks_UseCase3_StoreActivity.xlsx
+++ b/docs/DevTasks_UseCase3_StoreActivity.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$16</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>S.No.</t>
   </si>
@@ -57,7 +60,20 @@
 6. timeSpentInStore (save time in minutes, to be calculated only when storeEntryTime and storeExitTime are available)</t>
   </si>
   <si>
-    <t>Create a web service that takes following prameters in JSON format.
+    <t>Swarnima/Swapnil</t>
+  </si>
+  <si>
+    <t>Create service and dao classes to get loyal customers. The "storeActivity" item is to be queried to get the customers who visit stores the most</t>
+  </si>
+  <si>
+    <t>Customize product item type by adding following attribute.
+1. popularityCount (int type)</t>
+  </si>
+  <si>
+    <t>Create a one to many relation between beacon and products. And add some sample data in it (create impex)</t>
+  </si>
+  <si>
+    <t>Create a web service that takes following prameters in JSON format and save the data in hybris.
 1. storeId
 2. customerId
 3. storeVisitDate
@@ -66,22 +82,62 @@
 6. timeSpentInStore (save time in minutes, to be calculated only when storeEntryTime and storeExitTime are available)</t>
   </si>
   <si>
-    <t>Create service and dao classes to get most visited stores by customer. The "storeActivity" item is to be queried to get most visited stores</t>
-  </si>
-  <si>
-    <t>Swarnima/Swapnil</t>
-  </si>
-  <si>
-    <t>Create service and dao classes to get loyal customers. The "storeActivity" item is to be queried to get the customers who visit stores the most</t>
-  </si>
-  <si>
-    <t>18/03</t>
-  </si>
-  <si>
-    <t>20/03</t>
-  </si>
-  <si>
-    <t>19/03</t>
+    <t>Create service and dao classes to get top 5 popular products based on the popularity count. The count "5" should be made configurable.</t>
+  </si>
+  <si>
+    <t>23/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create an item "storeCustomer" and add following attributes to it.
+1. weight
+2. height
+3. Age
+4. Gender
+</t>
+  </si>
+  <si>
+    <t>Create a webservice to update the popularityCount of the product. The web service will accept the beaconId, majorId, minorId (in JSON format). Will use the request data to get the product from the relation defined in point 8 above and increase the popularity count for the product.</t>
+  </si>
+  <si>
+    <t>Create impex to store some sample data in storeCustomer point 11 above.</t>
+  </si>
+  <si>
+    <t>Create a WCMS page for the Activity dashboard, impex creation.</t>
+  </si>
+  <si>
+    <t>Create controller, facades, service classes to fetch model data for store customer profile section (point 11), popular products (based on product popularity count, point 7), most visited stores (point 4), loyal customers (from point 5), spent time (query storeActivity item, point 2)</t>
+  </si>
+  <si>
+    <t>To get weather information, there are two approaches. 
+1) The weather data is passed by IOS app, if so we can use it to dispplay on our page.
+2) To use java APIs to fetch weather data based on city or zip code. Please see the sample code http://code.aksingh.net/owm-japis/src</t>
+  </si>
+  <si>
+    <t>Create an item type "beacon" that contains following String type attributes.
+1. beaconId
+2. majorId
+3. minorId</t>
+  </si>
+  <si>
+    <t>24/03</t>
+  </si>
+  <si>
+    <t>25/03</t>
+  </si>
+  <si>
+    <t>27/03</t>
+  </si>
+  <si>
+    <t>30/03</t>
+  </si>
+  <si>
+    <t>26/03</t>
+  </si>
+  <si>
+    <t>31/03</t>
+  </si>
+  <si>
+    <t>Create service and dao classes to get most visited stores by customer. The "storeActivity" item (created in step 2) is to be queried to get most visited stores</t>
   </si>
 </sst>
 </file>
@@ -117,11 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -487,44 +544,44 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -532,19 +589,190 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>42095</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>42097</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>42097</v>
+      </c>
+      <c r="E13" s="2">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2">
+        <v>42096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>42097</v>
+      </c>
+      <c r="E16" s="2">
+        <v>42102</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated tasks for Use case 3
</commit_message>
<xml_diff>
--- a/docs/DevTasks_UseCase3_StoreActivity.xlsx
+++ b/docs/DevTasks_UseCase3_StoreActivity.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$22</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>S.No.</t>
   </si>
@@ -73,15 +73,6 @@
     <t>Create a one to many relation between beacon and products. And add some sample data in it (create impex)</t>
   </si>
   <si>
-    <t>Create a web service that takes following prameters in JSON format and save the data in hybris.
-1. storeId
-2. customerId
-3. storeVisitDate
-4. storeEntryTime
-5.storeExitTime
-6. timeSpentInStore (save time in minutes, to be calculated only when storeEntryTime and storeExitTime are available)</t>
-  </si>
-  <si>
     <t>Create service and dao classes to get top 5 popular products based on the popularity count. The count "5" should be made configurable.</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
 </t>
   </si>
   <si>
-    <t>Create a webservice to update the popularityCount of the product. The web service will accept the beaconId, majorId, minorId (in JSON format). Will use the request data to get the product from the relation defined in point 8 above and increase the popularity count for the product.</t>
-  </si>
-  <si>
     <t>Create impex to store some sample data in storeCustomer point 11 above.</t>
   </si>
   <si>
@@ -137,14 +125,70 @@
     <t>31/03</t>
   </si>
   <si>
-    <t>Create service and dao classes to get most visited stores by customer. The "storeActivity" item (created in step 2) is to be queried to get most visited stores</t>
+    <t>Create service and dao classes to get most visited stores by customers. The "storeActivity" item (created in step 2) is to be queried to get most visited stores</t>
+  </si>
+  <si>
+    <t>Property file - for showing a 5-6 most visited stores</t>
+  </si>
+  <si>
+    <t>Impex</t>
+  </si>
+  <si>
+    <t>Property file - for showing a 5-6 most loyal customers</t>
+  </si>
+  <si>
+    <t>Create some dummy data for storeActivity itemtype(Impex generation also)</t>
+  </si>
+  <si>
+    <t>Create an enumtype BeaconType with following Types
+1. Entry
+2. Exit
+3. Product
+4. Checkout</t>
+  </si>
+  <si>
+    <t>Create a relation between beacon and BeaconType, a one to many relation(create impex add some dummy data for beacons and relation)</t>
+  </si>
+  <si>
+    <t>Create dao, service classes for the above point</t>
+  </si>
+  <si>
+    <t>Create a web service which will return the status (status:entered/exited) in JSON format
+URL(/storeActivity)
+It will receive the following parameters:
+1. storeId
+2. customerId
+3. storeVisitDate</t>
+  </si>
+  <si>
+    <t>Create a webservice to update the popularityCount of the product. The web service will accept the beaconId, majorId, minorId (in JSON format).
+URL(/popularityCount)
+ Will use the request data to get the product from the relation defined in point 8 above and increase the popularity count for the product.</t>
+  </si>
+  <si>
+    <t>Create a webservice to return the beacon type in JSON format. The web service will accept the beaconId, majorId, minorId (in JSON format).
+URL(/beaconType)
+And it will query and return the type of the beacon</t>
+  </si>
+  <si>
+    <t>At the IOS side, we will need to have a link such that, when entry/exit beacon type is found, then they should send the webservice with URL /storeActivity
+When product beacon type is found then they should send the webservice with URL /popularityCount</t>
+  </si>
+  <si>
+    <t>First there will be a check whether the customer's entry exists, in case it exists and exit time is null in that, then it will calculate the timeSpentInStore and update the same along with the exit time.(as new Date())
+In case there is an entry and exit time is not null, also if there is no entry for the customer, then it will create a new entry and save the same along with the entry time (as new Date())
+calculate the following field in the controller method
+timeSpentInStore (save time in minutes, to be calculated only when storeEntryTime and storeExitTime are available)</t>
+  </si>
+  <si>
+    <t>Create service and dao classes for the above point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +196,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,17 +232,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,43 +546,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -527,13 +593,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,235 +610,293 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42095</v>
-      </c>
-      <c r="E11" s="2">
-        <v>42096</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2">
-        <v>42097</v>
-      </c>
-      <c r="E12" s="2">
-        <v>42097</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="2">
-        <v>42097</v>
-      </c>
-      <c r="E13" s="2">
-        <v>42097</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42095</v>
       </c>
       <c r="E15" s="2">
         <v>42096</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2">
+        <v>42097</v>
+      </c>
+      <c r="E18" s="2">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2">
+        <v>42097</v>
+      </c>
+      <c r="E19" s="2">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2">
+        <v>42096</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
         <v>42097</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E22" s="2">
         <v>42102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C16"/>
+  <autoFilter ref="C1:C22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>